<commit_message>
updates to OFFICE docs
updates to .docx and .xlsx files  to test binary files
</commit_message>
<xml_diff>
--- a/Vacation items checklist.xlsx
+++ b/Vacation items checklist.xlsx
@@ -111,9 +111,6 @@
     <t>Business Cards</t>
   </si>
   <si>
-    <t>Pre-Paid Phone Card</t>
-  </si>
-  <si>
     <t>Insect Repellent</t>
   </si>
   <si>
@@ -270,18 +267,12 @@
     <t>Re-Sealable Zipper Storage Bags</t>
   </si>
   <si>
-    <t>Hotel/ Accommodation Reservations</t>
-  </si>
-  <si>
     <t>Analgesic - Ibuprofen, Aspirin, etc.</t>
   </si>
   <si>
     <t>Bathing Suit &amp; Cover-up</t>
   </si>
   <si>
-    <t>Driver's License/International Driver's License</t>
-  </si>
-  <si>
     <t>Birth Certificates/Marriage License</t>
   </si>
   <si>
@@ -421,6 +412,15 @@
   </si>
   <si>
     <t>Vacation Items Checklist</t>
+  </si>
+  <si>
+    <t>Obtain Driver's License/International Driver's License</t>
+  </si>
+  <si>
+    <t>Premiere Hotel/ Accommodation Reservations</t>
+  </si>
+  <si>
+    <t>Pre-Paid Phone Card or prepaid mobile phone</t>
   </si>
 </sst>
 </file>
@@ -1881,7 +1881,9 @@
   </sheetPr>
   <dimension ref="B1:D125"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1895,7 +1897,7 @@
   <sheetData>
     <row r="1" spans="2:4" ht="108.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1917,7 +1919,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1928,7 +1930,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1937,7 +1939,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1946,7 +1948,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1957,7 +1959,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1966,7 +1968,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1986,7 +1988,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2015,7 +2017,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2024,7 +2026,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2033,7 +2035,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2042,7 +2044,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2051,7 +2053,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2069,7 +2071,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2078,7 +2080,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2087,7 +2089,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2105,7 +2107,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2114,7 +2116,7 @@
         <v>6</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2132,7 +2134,7 @@
         <v>6</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2141,7 +2143,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2150,7 +2152,7 @@
         <v>6</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2159,7 +2161,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2168,7 +2170,7 @@
         <v>6</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2177,7 +2179,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2186,7 +2188,7 @@
         <v>6</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2213,7 +2215,7 @@
         <v>6</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2222,7 +2224,7 @@
         <v>6</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2231,7 +2233,7 @@
         <v>6</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2240,7 +2242,7 @@
         <v>6</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2249,7 +2251,7 @@
         <v>6</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2258,7 +2260,7 @@
         <v>11</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2267,7 +2269,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2276,7 +2278,7 @@
         <v>11</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2285,7 +2287,7 @@
         <v>11</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2294,7 +2296,7 @@
         <v>11</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2303,7 +2305,7 @@
         <v>11</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2312,7 +2314,7 @@
         <v>11</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2321,7 +2323,7 @@
         <v>11</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2330,7 +2332,7 @@
         <v>11</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2339,7 +2341,7 @@
         <v>11</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2348,7 +2350,7 @@
         <v>12</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2357,7 +2359,7 @@
         <v>12</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2366,7 +2368,7 @@
         <v>12</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2375,7 +2377,7 @@
         <v>12</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2384,7 +2386,7 @@
         <v>12</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2393,7 +2395,7 @@
         <v>12</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2402,7 +2404,7 @@
         <v>12</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2411,7 +2413,7 @@
         <v>12</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2429,7 +2431,7 @@
         <v>12</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2438,7 +2440,7 @@
         <v>12</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2447,7 +2449,7 @@
         <v>12</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2465,7 +2467,7 @@
         <v>12</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2474,7 +2476,7 @@
         <v>12</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2483,7 +2485,7 @@
         <v>12</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2492,7 +2494,7 @@
         <v>12</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2501,7 +2503,7 @@
         <v>15</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2510,7 +2512,7 @@
         <v>15</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2519,7 +2521,7 @@
         <v>15</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2528,7 +2530,7 @@
         <v>15</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="72" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2537,7 +2539,7 @@
         <v>15</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2546,7 +2548,7 @@
         <v>15</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2555,7 +2557,7 @@
         <v>15</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2564,7 +2566,7 @@
         <v>15</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2573,7 +2575,7 @@
         <v>15</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2582,7 +2584,7 @@
         <v>15</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="78" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2591,7 +2593,7 @@
         <v>15</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2600,7 +2602,7 @@
         <v>15</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2609,7 +2611,7 @@
         <v>15</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2627,7 +2629,7 @@
         <v>15</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2636,7 +2638,7 @@
         <v>15</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2645,7 +2647,7 @@
         <v>15</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2654,7 +2656,7 @@
         <v>15</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2663,7 +2665,7 @@
         <v>15</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2672,7 +2674,7 @@
         <v>15</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="88" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2681,7 +2683,7 @@
         <v>15</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="89" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2699,7 +2701,7 @@
         <v>16</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="91" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2708,7 +2710,7 @@
         <v>16</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="92" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2717,7 +2719,7 @@
         <v>16</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="93" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2726,7 +2728,7 @@
         <v>16</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="94" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2735,7 +2737,7 @@
         <v>16</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="95" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2753,7 +2755,7 @@
         <v>16</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="97" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2762,7 +2764,7 @@
         <v>16</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="98" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2771,7 +2773,7 @@
         <v>16</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="99" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2780,7 +2782,7 @@
         <v>16</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2789,7 +2791,7 @@
         <v>16</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="101" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2798,7 +2800,7 @@
         <v>16</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="102" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2807,7 +2809,7 @@
         <v>16</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="103" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2816,7 +2818,7 @@
         <v>16</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="104" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2825,7 +2827,7 @@
         <v>16</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="105" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2843,7 +2845,7 @@
         <v>16</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="107" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2852,7 +2854,7 @@
         <v>16</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="108" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2861,7 +2863,7 @@
         <v>16</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="109" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2870,7 +2872,7 @@
         <v>16</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="110" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2879,7 +2881,7 @@
         <v>16</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="111" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2888,7 +2890,7 @@
         <v>16</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="112" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2906,7 +2908,7 @@
         <v>16</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="114" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2915,7 +2917,7 @@
         <v>16</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="115" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2924,7 +2926,7 @@
         <v>16</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="116" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2942,7 +2944,7 @@
         <v>16</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="118" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2951,7 +2953,7 @@
         <v>22</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="119" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2960,7 +2962,7 @@
         <v>22</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="120" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2969,7 +2971,7 @@
         <v>22</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2978,7 +2980,7 @@
         <v>22</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="122" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2987,7 +2989,7 @@
         <v>22</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="123" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2996,7 +2998,7 @@
         <v>22</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="124" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -3005,7 +3007,7 @@
         <v>22</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="125" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -3014,7 +3016,7 @@
         <v>22</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>